<commit_message>
add new terms to renewables EI
</commit_message>
<xml_diff>
--- a/concepts/renewables/input.xlsx
+++ b/concepts/renewables/input.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalyan/Documents/CPR/global-stocktake/concepts/renewables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234F790F-69C2-DF46-8E2B-EDC13E9B16E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB38F16B-3A08-1E47-9436-7AFDF5B27B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="Rule types" sheetId="2" r:id="rId2"/>
-    <sheet name="Entity types" sheetId="3" r:id="rId3"/>
+    <sheet name="new terms" sheetId="4" r:id="rId2"/>
+    <sheet name="Rule types" sheetId="2" r:id="rId3"/>
+    <sheet name="Entity types" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="227">
   <si>
     <t>Pattern name (optional)</t>
   </si>
@@ -522,12 +523,6 @@
     <t>farm</t>
   </si>
   <si>
-    <t>Wind project</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
     <t>Wind and solar</t>
   </si>
   <si>
@@ -594,6 +589,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> For any rules ending in _</t>
@@ -612,6 +608,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, values should be comma-separated. </t>
@@ -696,12 +693,75 @@
   <si>
     <t>https://spacy.io/models/en#en_core_web_sm-labels</t>
   </si>
+  <si>
+    <t>cane bagasse</t>
+  </si>
+  <si>
+    <t>harvest residues</t>
+  </si>
+  <si>
+    <t>heliothermic energy</t>
+  </si>
+  <si>
+    <t>Heliothermic</t>
+  </si>
+  <si>
+    <t>heliothermic</t>
+  </si>
+  <si>
+    <t>solar heat</t>
+  </si>
+  <si>
+    <t>marine</t>
+  </si>
+  <si>
+    <t>micro-hydraulic</t>
+  </si>
+  <si>
+    <t>micro</t>
+  </si>
+  <si>
+    <t>hydro,hydraulic</t>
+  </si>
+  <si>
+    <t>Ocean energy</t>
+  </si>
+  <si>
+    <t>ocean</t>
+  </si>
+  <si>
+    <t>renewable,thermal</t>
+  </si>
+  <si>
+    <t>ocean renewable energy, ocean thermal energy</t>
+  </si>
+  <si>
+    <t>otec</t>
+  </si>
+  <si>
+    <t>Wind parks</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>wind parks</t>
+  </si>
+  <si>
+    <t>project,resource</t>
+  </si>
+  <si>
+    <t>Wind project/resource</t>
+  </si>
+  <si>
+    <t>wind resource</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -763,6 +823,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -802,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -819,16 +886,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1047,10 +1115,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ1007"/>
+  <dimension ref="A1:AJ1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1064,16 +1132,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -1106,19 +1174,19 @@
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="Z1" s="11"/>
       <c r="AA1" s="11"/>
       <c r="AB1" s="11"/>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="14" t="s">
         <v>10</v>
       </c>
       <c r="AD1" s="11"/>
       <c r="AE1" s="11"/>
       <c r="AF1" s="11"/>
-      <c r="AG1" s="12" t="s">
+      <c r="AG1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="AH1" s="11"/>
@@ -3673,27 +3741,37 @@
     <row r="60" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>145</v>
+        <v>213</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="G60" s="5"/>
       <c r="I60" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L60" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M60" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J60" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="K60" s="5"/>
-      <c r="M60" s="5"/>
+      <c r="N60" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="O60" s="5"/>
       <c r="Q60" s="5"/>
       <c r="S60" s="5"/>
@@ -3715,20 +3793,25 @@
     <row r="61" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
       <c r="B61" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G61" s="5"/>
-      <c r="I61" s="5"/>
+      <c r="I61" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="K61" s="5"/>
       <c r="M61" s="5"/>
       <c r="O61" s="5"/>
@@ -3752,22 +3835,32 @@
     <row r="62" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="3"/>
       <c r="B62" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E62" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G62" s="5"/>
+      <c r="I62" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G62" s="5"/>
-      <c r="I62" s="5"/>
+      <c r="J62" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="K62" s="5"/>
-      <c r="M62" s="5"/>
+      <c r="M62" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N62" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="O62" s="5"/>
       <c r="Q62" s="5"/>
       <c r="S62" s="5"/>
@@ -3789,37 +3882,28 @@
     <row r="63" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="G63" s="5"/>
       <c r="I63" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K63" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L63" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M63" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N63" s="5" t="s">
-        <v>152</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="K63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
       <c r="O63" s="5"/>
       <c r="Q63" s="5"/>
       <c r="S63" s="5"/>
@@ -3841,22 +3925,32 @@
     <row r="64" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
       <c r="B64" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="G64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="I64" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="K64" s="5"/>
-      <c r="M64" s="5"/>
+      <c r="M64" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N64" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="O64" s="5"/>
       <c r="Q64" s="5"/>
       <c r="S64" s="5"/>
@@ -3878,27 +3972,24 @@
     <row r="65" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="3"/>
       <c r="B65" s="4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>155</v>
+        <v>220</v>
       </c>
       <c r="G65" s="5"/>
-      <c r="I65" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>139</v>
-      </c>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
       <c r="O65" s="5"/>
       <c r="Q65" s="5"/>
       <c r="S65" s="5"/>
@@ -3920,25 +4011,20 @@
     <row r="66" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G66" s="5"/>
-      <c r="I66" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>155</v>
-      </c>
+      <c r="I66" s="5"/>
       <c r="K66" s="5"/>
       <c r="M66" s="5"/>
       <c r="O66" s="5"/>
@@ -3962,37 +4048,22 @@
     <row r="67" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="G67" s="5"/>
-      <c r="I67" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K67" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L67" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M67" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N67" s="5" t="s">
-        <v>155</v>
-      </c>
+      <c r="I67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="M67" s="5"/>
       <c r="O67" s="5"/>
       <c r="Q67" s="5"/>
       <c r="S67" s="5"/>
@@ -4014,27 +4085,37 @@
     <row r="68" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="3"/>
       <c r="B68" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G68" s="5"/>
       <c r="I68" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M68" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J68" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="K68" s="5"/>
-      <c r="M68" s="5"/>
+      <c r="N68" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="O68" s="5"/>
       <c r="Q68" s="5"/>
       <c r="S68" s="5"/>
@@ -4056,37 +4137,22 @@
     <row r="69" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G69" s="5"/>
-      <c r="I69" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K69" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L69" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N69" s="5" t="s">
-        <v>155</v>
-      </c>
+      <c r="I69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="M69" s="5"/>
       <c r="O69" s="5"/>
       <c r="Q69" s="5"/>
       <c r="S69" s="5"/>
@@ -4108,24 +4174,24 @@
     <row r="70" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="3"/>
       <c r="B70" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>162</v>
+        <v>209</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>155</v>
+        <v>210</v>
       </c>
       <c r="G70" s="5"/>
       <c r="I70" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="K70" s="5"/>
       <c r="M70" s="5"/>
@@ -4154,7 +4220,7 @@
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>22</v>
@@ -4164,10 +4230,10 @@
       </c>
       <c r="G71" s="5"/>
       <c r="I71" s="5" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="K71" s="5"/>
       <c r="M71" s="5"/>
@@ -4196,24 +4262,23 @@
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G72" s="5"/>
       <c r="I72" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="K72" s="5"/>
       <c r="M72" s="5"/>
-      <c r="N72" s="5"/>
       <c r="O72" s="5"/>
       <c r="Q72" s="5"/>
       <c r="S72" s="5"/>
@@ -4239,27 +4304,32 @@
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F73" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G73" s="5"/>
+      <c r="I73" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L73" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N73" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="G73" s="5"/>
-      <c r="I73" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J73" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="K73" s="5"/>
-      <c r="M73" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N73" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="O73" s="5"/>
       <c r="Q73" s="5"/>
@@ -4282,32 +4352,27 @@
     <row r="74" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="3"/>
       <c r="B74" s="4" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G74" s="5"/>
       <c r="I74" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="K74" s="5"/>
-      <c r="M74" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N74" s="5" t="s">
-        <v>174</v>
-      </c>
+      <c r="M74" s="5"/>
       <c r="O74" s="5"/>
       <c r="Q74" s="5"/>
       <c r="S74" s="5"/>
@@ -4329,31 +4394,36 @@
     <row r="75" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="3"/>
       <c r="B75" s="4" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G75" s="5"/>
       <c r="I75" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="K75" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L75" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="M75" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="N75" s="5" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="O75" s="5"/>
       <c r="Q75" s="5"/>
@@ -4376,32 +4446,27 @@
     <row r="76" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="3"/>
       <c r="B76" s="4" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="G76" s="5"/>
       <c r="I76" s="5" t="s">
         <v>39</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="K76" s="5"/>
-      <c r="M76" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N76" s="5" t="s">
-        <v>174</v>
-      </c>
+      <c r="M76" s="5"/>
       <c r="O76" s="5"/>
       <c r="Q76" s="5"/>
       <c r="S76" s="5"/>
@@ -4423,40 +4488,32 @@
     <row r="77" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="3"/>
       <c r="B77" s="4" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C77" s="4"/>
-      <c r="D77" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E77" s="6" t="s">
+      <c r="D77" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F77" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
+      <c r="F77" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G77" s="5"/>
       <c r="I77" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J77" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
-      <c r="M77" s="6"/>
-      <c r="N77" s="6"/>
-      <c r="O77" s="6"/>
-      <c r="P77" s="6"/>
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
-      <c r="S77" s="6"/>
-      <c r="T77" s="6"/>
-      <c r="U77" s="6"/>
-      <c r="V77" s="6"/>
-      <c r="W77" s="6"/>
-      <c r="X77" s="6"/>
+      <c r="J77" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="Q77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="U77" s="5"/>
+      <c r="W77" s="5"/>
       <c r="Y77" s="6"/>
       <c r="Z77" s="6"/>
       <c r="AA77" s="6"/>
@@ -4473,40 +4530,32 @@
     <row r="78" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="3"/>
       <c r="B78" s="4" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="C78" s="4"/>
-      <c r="D78" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6" t="s">
+      <c r="D78" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J78" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6"/>
-      <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
-      <c r="S78" s="6"/>
-      <c r="T78" s="6"/>
-      <c r="U78" s="6"/>
-      <c r="V78" s="6"/>
-      <c r="W78" s="6"/>
-      <c r="X78" s="6"/>
+      <c r="F78" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G78" s="5"/>
+      <c r="I78" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="K78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="S78" s="5"/>
+      <c r="U78" s="5"/>
+      <c r="W78" s="5"/>
       <c r="Y78" s="6"/>
       <c r="Z78" s="6"/>
       <c r="AA78" s="6"/>
@@ -4522,29 +4571,34 @@
     </row>
     <row r="79" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="3"/>
-      <c r="B79" s="4"/>
+      <c r="B79" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="C79" s="4"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-      <c r="N79" s="6"/>
-      <c r="O79" s="6"/>
-      <c r="P79" s="6"/>
-      <c r="Q79" s="6"/>
-      <c r="R79" s="6"/>
-      <c r="S79" s="6"/>
-      <c r="T79" s="6"/>
-      <c r="U79" s="6"/>
-      <c r="V79" s="6"/>
-      <c r="W79" s="6"/>
-      <c r="X79" s="6"/>
+      <c r="D79" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G79" s="5"/>
+      <c r="I79" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="K79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="S79" s="5"/>
+      <c r="U79" s="5"/>
+      <c r="W79" s="5"/>
       <c r="Y79" s="6"/>
       <c r="Z79" s="6"/>
       <c r="AA79" s="6"/>
@@ -4560,29 +4614,38 @@
     </row>
     <row r="80" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
-      <c r="B80" s="4"/>
+      <c r="B80" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="C80" s="4"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="6"/>
-      <c r="P80" s="6"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="6"/>
-      <c r="S80" s="6"/>
-      <c r="T80" s="6"/>
-      <c r="U80" s="6"/>
-      <c r="V80" s="6"/>
-      <c r="W80" s="6"/>
-      <c r="X80" s="6"/>
+      <c r="D80" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G80" s="5"/>
+      <c r="I80" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K80" s="5"/>
+      <c r="M80" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N80" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="O80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="S80" s="5"/>
+      <c r="U80" s="5"/>
+      <c r="W80" s="5"/>
       <c r="Y80" s="6"/>
       <c r="Z80" s="6"/>
       <c r="AA80" s="6"/>
@@ -4598,14 +4661,33 @@
     </row>
     <row r="81" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="3"/>
-      <c r="B81" s="4"/>
+      <c r="B81" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="5"/>
+      <c r="D81" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="G81" s="5"/>
-      <c r="I81" s="5"/>
+      <c r="I81" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="K81" s="5"/>
-      <c r="M81" s="5"/>
+      <c r="M81" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N81" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="O81" s="5"/>
       <c r="Q81" s="5"/>
       <c r="S81" s="5"/>
@@ -4626,14 +4708,33 @@
     </row>
     <row r="82" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="3"/>
-      <c r="B82" s="4"/>
+      <c r="B82" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="5"/>
+      <c r="D82" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="G82" s="5"/>
-      <c r="I82" s="5"/>
+      <c r="I82" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="K82" s="5"/>
-      <c r="M82" s="5"/>
+      <c r="M82" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N82" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="O82" s="5"/>
       <c r="Q82" s="5"/>
       <c r="S82" s="5"/>
@@ -4654,14 +4755,33 @@
     </row>
     <row r="83" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="3"/>
-      <c r="B83" s="4"/>
+      <c r="B83" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="5"/>
+      <c r="D83" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="G83" s="5"/>
-      <c r="I83" s="5"/>
+      <c r="I83" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="K83" s="5"/>
-      <c r="M83" s="5"/>
+      <c r="M83" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="O83" s="5"/>
       <c r="Q83" s="5"/>
       <c r="S83" s="5"/>
@@ -4682,19 +4802,41 @@
     </row>
     <row r="84" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="3"/>
-      <c r="B84" s="4"/>
+      <c r="B84" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="K84" s="5"/>
-      <c r="M84" s="5"/>
-      <c r="O84" s="5"/>
-      <c r="Q84" s="5"/>
-      <c r="S84" s="5"/>
-      <c r="U84" s="5"/>
-      <c r="W84" s="5"/>
+      <c r="D84" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J84" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="6"/>
+      <c r="Q84" s="6"/>
+      <c r="R84" s="6"/>
+      <c r="S84" s="6"/>
+      <c r="T84" s="6"/>
+      <c r="U84" s="6"/>
+      <c r="V84" s="6"/>
+      <c r="W84" s="6"/>
+      <c r="X84" s="6"/>
       <c r="Y84" s="6"/>
       <c r="Z84" s="6"/>
       <c r="AA84" s="6"/>
@@ -4710,19 +4852,41 @@
     </row>
     <row r="85" spans="1:36" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="3"/>
-      <c r="B85" s="4"/>
+      <c r="B85" s="4" t="s">
+        <v>179</v>
+      </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="I85" s="5"/>
-      <c r="K85" s="5"/>
-      <c r="M85" s="5"/>
-      <c r="O85" s="5"/>
-      <c r="Q85" s="5"/>
-      <c r="S85" s="5"/>
-      <c r="U85" s="5"/>
-      <c r="W85" s="5"/>
+      <c r="D85" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J85" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="6"/>
+      <c r="T85" s="6"/>
+      <c r="U85" s="6"/>
+      <c r="V85" s="6"/>
+      <c r="W85" s="6"/>
+      <c r="X85" s="6"/>
       <c r="Y85" s="6"/>
       <c r="Z85" s="6"/>
       <c r="AA85" s="6"/>
@@ -4740,17 +4904,27 @@
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="I86" s="5"/>
-      <c r="K86" s="5"/>
-      <c r="M86" s="5"/>
-      <c r="O86" s="5"/>
-      <c r="Q86" s="5"/>
-      <c r="S86" s="5"/>
-      <c r="U86" s="5"/>
-      <c r="W86" s="5"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="6"/>
+      <c r="T86" s="6"/>
+      <c r="U86" s="6"/>
+      <c r="V86" s="6"/>
+      <c r="W86" s="6"/>
+      <c r="X86" s="6"/>
       <c r="Y86" s="6"/>
       <c r="Z86" s="6"/>
       <c r="AA86" s="6"/>
@@ -4768,17 +4942,27 @@
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="5"/>
-      <c r="G87" s="5"/>
-      <c r="I87" s="5"/>
-      <c r="K87" s="5"/>
-      <c r="M87" s="5"/>
-      <c r="O87" s="5"/>
-      <c r="Q87" s="5"/>
-      <c r="S87" s="5"/>
-      <c r="U87" s="5"/>
-      <c r="W87" s="5"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+      <c r="Q87" s="6"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="6"/>
+      <c r="T87" s="6"/>
+      <c r="U87" s="6"/>
+      <c r="V87" s="6"/>
+      <c r="W87" s="6"/>
+      <c r="X87" s="6"/>
       <c r="Y87" s="6"/>
       <c r="Z87" s="6"/>
       <c r="AA87" s="6"/>
@@ -30552,8 +30736,209 @@
       <c r="AI1007" s="6"/>
       <c r="AJ1007" s="6"/>
     </row>
+    <row r="1008" spans="1:36" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1008" s="3"/>
+      <c r="B1008" s="4"/>
+      <c r="C1008" s="4"/>
+      <c r="D1008" s="4"/>
+      <c r="E1008" s="5"/>
+      <c r="G1008" s="5"/>
+      <c r="I1008" s="5"/>
+      <c r="K1008" s="5"/>
+      <c r="M1008" s="5"/>
+      <c r="O1008" s="5"/>
+      <c r="Q1008" s="5"/>
+      <c r="S1008" s="5"/>
+      <c r="U1008" s="5"/>
+      <c r="W1008" s="5"/>
+      <c r="Y1008" s="6"/>
+      <c r="Z1008" s="6"/>
+      <c r="AA1008" s="6"/>
+      <c r="AB1008" s="6"/>
+      <c r="AC1008" s="6"/>
+      <c r="AD1008" s="6"/>
+      <c r="AE1008" s="6"/>
+      <c r="AF1008" s="6"/>
+      <c r="AG1008" s="6"/>
+      <c r="AH1008" s="6"/>
+      <c r="AI1008" s="6"/>
+      <c r="AJ1008" s="6"/>
+    </row>
+    <row r="1009" spans="1:36" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1009" s="3"/>
+      <c r="B1009" s="4"/>
+      <c r="C1009" s="4"/>
+      <c r="D1009" s="4"/>
+      <c r="E1009" s="5"/>
+      <c r="G1009" s="5"/>
+      <c r="I1009" s="5"/>
+      <c r="K1009" s="5"/>
+      <c r="M1009" s="5"/>
+      <c r="O1009" s="5"/>
+      <c r="Q1009" s="5"/>
+      <c r="S1009" s="5"/>
+      <c r="U1009" s="5"/>
+      <c r="W1009" s="5"/>
+      <c r="Y1009" s="6"/>
+      <c r="Z1009" s="6"/>
+      <c r="AA1009" s="6"/>
+      <c r="AB1009" s="6"/>
+      <c r="AC1009" s="6"/>
+      <c r="AD1009" s="6"/>
+      <c r="AE1009" s="6"/>
+      <c r="AF1009" s="6"/>
+      <c r="AG1009" s="6"/>
+      <c r="AH1009" s="6"/>
+      <c r="AI1009" s="6"/>
+      <c r="AJ1009" s="6"/>
+    </row>
+    <row r="1010" spans="1:36" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1010" s="3"/>
+      <c r="B1010" s="4"/>
+      <c r="C1010" s="4"/>
+      <c r="D1010" s="4"/>
+      <c r="E1010" s="5"/>
+      <c r="G1010" s="5"/>
+      <c r="I1010" s="5"/>
+      <c r="K1010" s="5"/>
+      <c r="M1010" s="5"/>
+      <c r="O1010" s="5"/>
+      <c r="Q1010" s="5"/>
+      <c r="S1010" s="5"/>
+      <c r="U1010" s="5"/>
+      <c r="W1010" s="5"/>
+      <c r="Y1010" s="6"/>
+      <c r="Z1010" s="6"/>
+      <c r="AA1010" s="6"/>
+      <c r="AB1010" s="6"/>
+      <c r="AC1010" s="6"/>
+      <c r="AD1010" s="6"/>
+      <c r="AE1010" s="6"/>
+      <c r="AF1010" s="6"/>
+      <c r="AG1010" s="6"/>
+      <c r="AH1010" s="6"/>
+      <c r="AI1010" s="6"/>
+      <c r="AJ1010" s="6"/>
+    </row>
+    <row r="1011" spans="1:36" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1011" s="3"/>
+      <c r="B1011" s="4"/>
+      <c r="C1011" s="4"/>
+      <c r="D1011" s="4"/>
+      <c r="E1011" s="5"/>
+      <c r="G1011" s="5"/>
+      <c r="I1011" s="5"/>
+      <c r="K1011" s="5"/>
+      <c r="M1011" s="5"/>
+      <c r="O1011" s="5"/>
+      <c r="Q1011" s="5"/>
+      <c r="S1011" s="5"/>
+      <c r="U1011" s="5"/>
+      <c r="W1011" s="5"/>
+      <c r="Y1011" s="6"/>
+      <c r="Z1011" s="6"/>
+      <c r="AA1011" s="6"/>
+      <c r="AB1011" s="6"/>
+      <c r="AC1011" s="6"/>
+      <c r="AD1011" s="6"/>
+      <c r="AE1011" s="6"/>
+      <c r="AF1011" s="6"/>
+      <c r="AG1011" s="6"/>
+      <c r="AH1011" s="6"/>
+      <c r="AI1011" s="6"/>
+      <c r="AJ1011" s="6"/>
+    </row>
+    <row r="1012" spans="1:36" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1012" s="3"/>
+      <c r="B1012" s="4"/>
+      <c r="C1012" s="4"/>
+      <c r="D1012" s="4"/>
+      <c r="E1012" s="5"/>
+      <c r="G1012" s="5"/>
+      <c r="I1012" s="5"/>
+      <c r="K1012" s="5"/>
+      <c r="M1012" s="5"/>
+      <c r="O1012" s="5"/>
+      <c r="Q1012" s="5"/>
+      <c r="S1012" s="5"/>
+      <c r="U1012" s="5"/>
+      <c r="W1012" s="5"/>
+      <c r="Y1012" s="6"/>
+      <c r="Z1012" s="6"/>
+      <c r="AA1012" s="6"/>
+      <c r="AB1012" s="6"/>
+      <c r="AC1012" s="6"/>
+      <c r="AD1012" s="6"/>
+      <c r="AE1012" s="6"/>
+      <c r="AF1012" s="6"/>
+      <c r="AG1012" s="6"/>
+      <c r="AH1012" s="6"/>
+      <c r="AI1012" s="6"/>
+      <c r="AJ1012" s="6"/>
+    </row>
+    <row r="1013" spans="1:36" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1013" s="3"/>
+      <c r="B1013" s="4"/>
+      <c r="C1013" s="4"/>
+      <c r="D1013" s="4"/>
+      <c r="E1013" s="5"/>
+      <c r="G1013" s="5"/>
+      <c r="I1013" s="5"/>
+      <c r="K1013" s="5"/>
+      <c r="M1013" s="5"/>
+      <c r="O1013" s="5"/>
+      <c r="Q1013" s="5"/>
+      <c r="S1013" s="5"/>
+      <c r="U1013" s="5"/>
+      <c r="W1013" s="5"/>
+      <c r="Y1013" s="6"/>
+      <c r="Z1013" s="6"/>
+      <c r="AA1013" s="6"/>
+      <c r="AB1013" s="6"/>
+      <c r="AC1013" s="6"/>
+      <c r="AD1013" s="6"/>
+      <c r="AE1013" s="6"/>
+      <c r="AF1013" s="6"/>
+      <c r="AG1013" s="6"/>
+      <c r="AH1013" s="6"/>
+      <c r="AI1013" s="6"/>
+      <c r="AJ1013" s="6"/>
+    </row>
+    <row r="1014" spans="1:36" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1014" s="3"/>
+      <c r="B1014" s="4"/>
+      <c r="C1014" s="4"/>
+      <c r="D1014" s="4"/>
+      <c r="E1014" s="5"/>
+      <c r="G1014" s="5"/>
+      <c r="I1014" s="5"/>
+      <c r="K1014" s="5"/>
+      <c r="M1014" s="5"/>
+      <c r="O1014" s="5"/>
+      <c r="Q1014" s="5"/>
+      <c r="S1014" s="5"/>
+      <c r="U1014" s="5"/>
+      <c r="W1014" s="5"/>
+      <c r="Y1014" s="6"/>
+      <c r="Z1014" s="6"/>
+      <c r="AA1014" s="6"/>
+      <c r="AB1014" s="6"/>
+      <c r="AC1014" s="6"/>
+      <c r="AD1014" s="6"/>
+      <c r="AE1014" s="6"/>
+      <c r="AF1014" s="6"/>
+      <c r="AG1014" s="6"/>
+      <c r="AH1014" s="6"/>
+      <c r="AI1014" s="6"/>
+      <c r="AJ1014" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="A1:A2"/>
@@ -30561,11 +30946,6 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AJ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -30576,7 +30956,7 @@
           <x14:formula1>
             <xm:f>'Rule types'!$A$3:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>AI3:AI1007 AG3:AG1007 AE3:AE1007 AC3:AC1007 AA3:AA1007 Y3:Y1007 W3:W1007 U3:U1007 S3:S1007 Q3:Q1007 O3:O1007 M3:M1007 K3:K1007 I3:I1007 G3:G1007 E3:E1007</xm:sqref>
+          <xm:sqref>I3:I1014 G3:G1014 E3:E1014 AG3:AG1014 AE3:AE1014 AC3:AC1014 AA3:AA1014 Y3:Y1014 W3:W1014 U3:U1014 S3:S1014 Q3:Q1014 O3:O1014 K3:K1014 AI3:AI1014 M3:M1014</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -30585,6 +30965,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C870A3-B335-6241-A361-5E8A54147CD2}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -30597,7 +31037,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -30617,12 +31057,12 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -30632,27 +31072,27 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -30662,67 +31102,67 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -30732,7 +31172,7 @@
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -30747,7 +31187,7 @@
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -30761,7 +31201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -30774,7 +31214,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>